<commit_message>
cleaned up fitting spreadsheets
</commit_message>
<xml_diff>
--- a/compiled_data/296_303_LGQTSVDR_fitting.xlsx
+++ b/compiled_data/296_303_LGQTSVDR_fitting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anumglasgow/Dropbox/Research/Data/HDX/20200922_compile_rates/compiled_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B927E70-B8DB-6D4F-9B0F-13CBD55DFBF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7985495B-9288-964C-87D5-6D0C601FBF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="600" windowWidth="21940" windowHeight="13900" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Peptide SD" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -560,7 +559,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:AX35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>